<commit_message>
Testing new drone data points and impact data
</commit_message>
<xml_diff>
--- a/Drone_Data_Code/Drone Data New Points.xlsx
+++ b/Drone_Data_Code/Drone Data New Points.xlsx
@@ -447,82 +447,82 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>468.9871372456365</v>
+        <v>422.1640277809471</v>
       </c>
       <c r="B2" t="n">
-        <v>87.24780837981224</v>
+        <v>72.29138580545695</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>454.2750648876533</v>
+        <v>434.0774227789693</v>
       </c>
       <c r="B3" t="n">
-        <v>96.1877149045562</v>
+        <v>68.84493981932113</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>469.0185420548063</v>
+        <v>438.4150340832591</v>
       </c>
       <c r="B4" t="n">
-        <v>99.10593022292586</v>
+        <v>70.97626561410722</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>462.7206844754957</v>
+        <v>431.0540579015487</v>
       </c>
       <c r="B5" t="n">
-        <v>91.44546161527342</v>
+        <v>68.03717310698939</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>372.6575061592242</v>
+        <v>438.7164927469763</v>
       </c>
       <c r="B6" t="n">
-        <v>144.1020925920716</v>
+        <v>54.37358433650676</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>408.0970831685067</v>
+        <v>435.4090084474875</v>
       </c>
       <c r="B7" t="n">
-        <v>146.4778599029966</v>
+        <v>79.80926178634144</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>465.6123448749435</v>
+        <v>421.0657516171254</v>
       </c>
       <c r="B8" t="n">
-        <v>103.9500741829945</v>
+        <v>69.26105417588337</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>360.4414395061177</v>
+        <v>409.926635397423</v>
       </c>
       <c r="B9" t="n">
-        <v>133.6781432058789</v>
+        <v>56.87163956602839</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>389.8996751719276</v>
+        <v>439.215700756011</v>
       </c>
       <c r="B10" t="n">
-        <v>138.7856313296645</v>
+        <v>57.72587477486562</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>394.8560535070105</v>
+        <v>432.7363602554482</v>
       </c>
       <c r="B11" t="n">
-        <v>136.1475278490561</v>
+        <v>74.92266025006445</v>
       </c>
     </row>
   </sheetData>

</xml_diff>